<commit_message>
post power consumption testing
</commit_message>
<xml_diff>
--- a/Testing/power consumption.xlsx
+++ b/Testing/power consumption.xlsx
@@ -24,12 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>mA</t>
   </si>
   <si>
     <t>Clock Speed MHz</t>
+  </si>
+  <si>
+    <t>using TPS54302</t>
+  </si>
+  <si>
+    <t>mhz</t>
+  </si>
+  <si>
+    <t>ma</t>
   </si>
 </sst>
 </file>
@@ -226,11 +235,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="6644736"/>
-        <c:axId val="6645128"/>
+        <c:axId val="402614264"/>
+        <c:axId val="402614648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="6644736"/>
+        <c:axId val="402614264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -287,12 +296,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6645128"/>
+        <c:crossAx val="402614648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="6645128"/>
+        <c:axId val="402614648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -349,7 +358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6644736"/>
+        <c:crossAx val="402614264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1252,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,6 +1328,51 @@
         <v>81</v>
       </c>
     </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>6.37</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>11.99</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>96</v>
+      </c>
+      <c r="C15">
+        <v>21.97</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="B3:C8">
     <sortCondition ref="C3:C8"/>

</xml_diff>